<commit_message>
Kinda got bottom-sku eligibility working; needs more work
</commit_message>
<xml_diff>
--- a/data_jul4/SO-PackExport Data_Shortened.xlsx
+++ b/data_jul4/SO-PackExport Data_Shortened.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\braed\source\repos\Bundle_Optimization\data_jul4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\Source\bundle-optimization-new\data_jul4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B99A2A21-23F3-4B0B-8290-3FC9E3EDAB86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D661CA-7BC1-411E-8CFE-D79904C8E454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SO-PackExportData" sheetId="3" r:id="rId1"/>
@@ -24,8 +24,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -724,56 +722,55 @@
   <dimension ref="A1:AP31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="F4" sqref="F4:F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="75.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="41.21875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="36.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="75.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="41.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="36.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8.5546875" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="12.77734375" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="7.5546875" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="28" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -901,7 +898,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -1017,7 +1014,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>41</v>
       </c>
@@ -1133,7 +1130,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>41</v>
       </c>
@@ -1249,7 +1246,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>41</v>
       </c>
@@ -1365,7 +1362,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
@@ -1481,7 +1478,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -1597,7 +1594,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
@@ -1713,7 +1710,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>41</v>
       </c>
@@ -1829,7 +1826,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>41</v>
       </c>
@@ -1945,7 +1942,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>41</v>
       </c>
@@ -2064,7 +2061,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>41</v>
       </c>
@@ -2180,7 +2177,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -2296,7 +2293,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -2412,7 +2409,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>41</v>
       </c>
@@ -2528,7 +2525,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -2644,7 +2641,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -2760,7 +2757,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>41</v>
       </c>
@@ -2876,7 +2873,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="19" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>41</v>
       </c>
@@ -2992,7 +2989,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="20" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -3108,7 +3105,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>41</v>
       </c>
@@ -3224,7 +3221,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>41</v>
       </c>
@@ -3340,7 +3337,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -3456,7 +3453,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="24" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>41</v>
       </c>
@@ -3572,7 +3569,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="25" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>41</v>
       </c>
@@ -3688,7 +3685,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>41</v>
       </c>
@@ -3804,7 +3801,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>41</v>
       </c>
@@ -3920,7 +3917,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>41</v>
       </c>
@@ -4036,7 +4033,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="29" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>41</v>
       </c>
@@ -4152,7 +4149,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>41</v>
       </c>
@@ -4268,7 +4265,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="31" spans="1:42" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:42" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>41</v>
       </c>

</xml_diff>

<commit_message>
Finished everything, filler on inside is the only thing to go
</commit_message>
<xml_diff>
--- a/data_jul4/SO-PackExport Data_Shortened.xlsx
+++ b/data_jul4/SO-PackExport Data_Shortened.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\McRae\Source\bundle-optimization-new\data_jul4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00D661CA-7BC1-411E-8CFE-D79904C8E454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D845D8-BC4D-4C39-A141-F51CCC51B335}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -722,7 +722,7 @@
   <dimension ref="A1:AP31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4:F5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1146,7 +1146,9 @@
       <c r="E4" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2">
+        <v>1</v>
+      </c>
       <c r="G4" s="2" t="s">
         <v>62</v>
       </c>
@@ -1262,7 +1264,9 @@
       <c r="E5" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="F5" s="2"/>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
       <c r="G5" s="2" t="s">
         <v>64</v>
       </c>

</xml_diff>